<commit_message>
updates to MC and alignment
</commit_message>
<xml_diff>
--- a/Data_paper/Aligment Simulations/par_alignment.xlsx
+++ b/Data_paper/Aligment Simulations/par_alignment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\GitHub\CaliAli\Data_paper\Aligment Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CFC627-F4ED-42C0-8088-081DF7EE383E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6409E0C6-7098-4013-8D2D-85ED598B01F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="48" windowWidth="29304" windowHeight="13632" xr2:uid="{AF3DAF21-7C39-47B8-8585-A48E26BCD7C4}"/>
+    <workbookView xWindow="14664" yWindow="0" windowWidth="24780" windowHeight="13632" xr2:uid="{AF3DAF21-7C39-47B8-8585-A48E26BCD7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="8">
   <si>
     <t>motion</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>save_files</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -416,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D5212D-FA8B-4711-97C2-C6774381873D}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L40"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33:N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -467,8 +470,14 @@
       <c r="N1">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -511,8 +520,14 @@
       <c r="N2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -555,8 +570,14 @@
       <c r="N3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -599,8 +620,14 @@
       <c r="N4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O4" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -643,8 +670,14 @@
       <c r="N5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -687,8 +720,14 @@
       <c r="N6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -731,8 +770,14 @@
       <c r="N7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -775,8 +820,14 @@
       <c r="N8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O8" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -819,8 +870,14 @@
       <c r="N9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O9" t="s">
+        <v>7</v>
+      </c>
+      <c r="P9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -863,8 +920,14 @@
       <c r="N10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -907,8 +970,14 @@
       <c r="N11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O11" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -951,8 +1020,14 @@
       <c r="N12">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O12" t="s">
+        <v>7</v>
+      </c>
+      <c r="P12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -995,8 +1070,14 @@
       <c r="N13">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O13" t="s">
+        <v>7</v>
+      </c>
+      <c r="P13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1039,8 +1120,14 @@
       <c r="N14">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>7</v>
+      </c>
+      <c r="P14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1083,8 +1170,14 @@
       <c r="N15">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O15" t="s">
+        <v>7</v>
+      </c>
+      <c r="P15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1127,8 +1220,14 @@
       <c r="N16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O16" t="s">
+        <v>7</v>
+      </c>
+      <c r="P16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1171,8 +1270,14 @@
       <c r="N17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O17" t="s">
+        <v>7</v>
+      </c>
+      <c r="P17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1215,8 +1320,14 @@
       <c r="N18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O18" t="s">
+        <v>7</v>
+      </c>
+      <c r="P18">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1259,8 +1370,14 @@
       <c r="N19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O19" t="s">
+        <v>7</v>
+      </c>
+      <c r="P19">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1303,8 +1420,14 @@
       <c r="N20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1347,8 +1470,14 @@
       <c r="N21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>7</v>
+      </c>
+      <c r="P21">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1391,8 +1520,14 @@
       <c r="N22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O22" t="s">
+        <v>7</v>
+      </c>
+      <c r="P22">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1435,8 +1570,14 @@
       <c r="N23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O23" t="s">
+        <v>7</v>
+      </c>
+      <c r="P23">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1479,8 +1620,14 @@
       <c r="N24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O24" t="s">
+        <v>7</v>
+      </c>
+      <c r="P24">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1523,8 +1670,14 @@
       <c r="N25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O25" t="s">
+        <v>7</v>
+      </c>
+      <c r="P25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1567,8 +1720,14 @@
       <c r="N26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O26" t="s">
+        <v>7</v>
+      </c>
+      <c r="P26">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1611,8 +1770,14 @@
       <c r="N27">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O27" t="s">
+        <v>7</v>
+      </c>
+      <c r="P27">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1655,8 +1820,14 @@
       <c r="N28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O28" t="s">
+        <v>7</v>
+      </c>
+      <c r="P28">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1699,8 +1870,14 @@
       <c r="N29">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O29" t="s">
+        <v>7</v>
+      </c>
+      <c r="P29">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1743,8 +1920,14 @@
       <c r="N30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O30" t="s">
+        <v>7</v>
+      </c>
+      <c r="P30">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1787,8 +1970,14 @@
       <c r="N31">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O31" t="s">
+        <v>7</v>
+      </c>
+      <c r="P31">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1831,8 +2020,14 @@
       <c r="N32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O32" t="s">
+        <v>7</v>
+      </c>
+      <c r="P32">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1875,8 +2070,14 @@
       <c r="N33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O33" t="s">
+        <v>7</v>
+      </c>
+      <c r="P33">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1919,8 +2120,14 @@
       <c r="N34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O34" t="s">
+        <v>7</v>
+      </c>
+      <c r="P34">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1963,8 +2170,14 @@
       <c r="N35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O35" t="s">
+        <v>7</v>
+      </c>
+      <c r="P35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -2007,8 +2220,14 @@
       <c r="N36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O36" t="s">
+        <v>7</v>
+      </c>
+      <c r="P36">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -2051,8 +2270,14 @@
       <c r="N37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O37" t="s">
+        <v>7</v>
+      </c>
+      <c r="P37">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -2095,8 +2320,14 @@
       <c r="N38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O38" t="s">
+        <v>7</v>
+      </c>
+      <c r="P38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -2139,8 +2370,14 @@
       <c r="N39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O39" t="s">
+        <v>7</v>
+      </c>
+      <c r="P39">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -2182,10 +2419,17 @@
       </c>
       <c r="N40">
         <v>2</v>
+      </c>
+      <c r="O40" t="s">
+        <v>7</v>
+      </c>
+      <c r="P40">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>